<commit_message>
problem on majority element 2
</commit_message>
<xml_diff>
--- a/Practice_Tracker.xlsx
+++ b/Practice_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanthsairambhatlapenumarthi/Documents/DSA_Practice/Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5487E4-F1AD-A241-A838-5AE92A862FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A19EC48-3AD4-D649-8E4B-DFFD800B28BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{FECDC1C9-E069-6A41-B650-1E342BB5A116}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Rotate Array</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=7pnhv842keE</t>
+  </si>
+  <si>
+    <t>majority element 2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Eua-UrQ_ANo</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Need to revisit , understood problem partially 😭</t>
+  </si>
+  <si>
+    <t>Ok, I'm clear with the problem</t>
   </si>
 </sst>
 </file>
@@ -190,8 +205,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D02FD38B-9928-CA4A-ADDB-16F1FDCC62FF}" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0">
-  <autoFilter ref="A1:H6" xr:uid="{D02FD38B-9928-CA4A-ADDB-16F1FDCC62FF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D02FD38B-9928-CA4A-ADDB-16F1FDCC62FF}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0">
+  <autoFilter ref="A1:I7" xr:uid="{D02FD38B-9928-CA4A-ADDB-16F1FDCC62FF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -200,8 +215,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C390EF8F-DF66-584C-BE6E-E6FE3CAEF6B6}" name="s. no" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{4C7210CB-05C0-7F4A-92C3-03D27163101C}" name="Problems" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{EF29F300-ACBE-AF46-9A62-B69B239C2904}" name="Complexity Level"/>
@@ -210,6 +226,7 @@
     <tableColumn id="6" xr3:uid="{389ADEF2-4860-5E40-A605-F32AD9A2CB12}" name="Notes/ resources"/>
     <tableColumn id="7" xr3:uid="{1A1F0075-3861-6B46-BEDE-674AFE9CDB64}" name="Practise count"/>
     <tableColumn id="8" xr3:uid="{3D5ABD18-CC08-9C44-84FC-329436D0DF71}" name="Confidence Level (1-5)"/>
+    <tableColumn id="9" xr3:uid="{46EE5E58-B205-CE44-BE0B-F50C4EB87803}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C1A419-B78B-6B40-8632-0244C2547F01}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -546,9 +563,10 @@
     <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -573,8 +591,11 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -599,8 +620,11 @@
       <c r="H2">
         <v>3</v>
       </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -625,8 +649,11 @@
       <c r="H3">
         <v>2</v>
       </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -651,8 +678,11 @@
       <c r="H4">
         <v>4</v>
       </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -677,8 +707,11 @@
       <c r="H5">
         <v>4</v>
       </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -702,6 +735,38 @@
       </c>
       <c r="H6">
         <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45906</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -718,16 +783,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{96A3533A-028B-4841-B48A-3CA8EDFFDB5C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7" xr:uid="{96A3533A-028B-4841-B48A-3CA8EDFFDB5C}">
       <formula1>"Easy,Medium,Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{A2374E35-0CD7-974D-8A9E-F0A340700751}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{A2374E35-0CD7-974D-8A9E-F0A340700751}">
       <formula1>"Completed, Stuck, In-Progress, Not-yet started"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{0F5D519C-68F7-C942-AD46-E98E68DE42A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{0F5D519C-68F7-C942-AD46-E98E68DE42A5}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{F92C85C4-2FE7-384A-B3F9-7508D61A7998}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{F92C85C4-2FE7-384A-B3F9-7508D61A7998}">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -737,10 +802,12 @@
     <hyperlink ref="B5" r:id="rId3" display="https://leetcode.com/problems/maximum-product-subarray/" xr:uid="{711709E3-B18F-D24A-86A2-F717ACD66A53}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{3314A5F6-C96D-8049-8263-33B7F07A0D6A}"/>
     <hyperlink ref="B6" r:id="rId5" display="https://leetcode.com/problems/majority-element/" xr:uid="{377D2CA8-2F80-3B48-BDFB-1369D0DEAFFE}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://leetcode.com/problems/majority-element-ii/" xr:uid="{5FC79E88-82A4-A440-A8ED-F08D6649FCC6}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{2B395BBD-0618-BF4A-8E91-CA87BF4393D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>